<commit_message>
Add interview and survey
</commit_message>
<xml_diff>
--- a/docs/Armenian youth questionnaire on spiritual life series pilot (Responses).xlsx
+++ b/docs/Armenian youth questionnaire on spiritual life series pilot (Responses).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ArenBabikian.github.io\gantegh\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sourphagopyouth\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC56170-58F8-4E9E-9EF8-AD34B3A21ECC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E682B72-9E3A-4164-9B5A-8F03E755FC2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4155" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4995" yWindow="2880" windowWidth="22845" windowHeight="11595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -540,10 +540,54 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.30057493540051677"/>
-                  <c:y val="-0.14351862943465912"/>
+                  <c:x val="-0.10747543859649122"/>
+                  <c:y val="-8.1987726098191216E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{5E8CB431-7664-4F5C-97EF-7365DBE5727C}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>;</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:fld id="{02F3DFAA-ACBA-4621-AC83-3324A6F7A5ED}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -601,8 +645,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 164207"/>
-                        <a:gd name="adj2" fmla="val -54410"/>
+                        <a:gd name="adj1" fmla="val 81531"/>
+                        <a:gd name="adj2" fmla="val -107888"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -623,6 +667,8 @@
                       <a:noFill/>
                     </a:ln>
                   </c15:spPr>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-12CE-4448-BD84-2EB2E274863D}"/>
@@ -633,10 +679,54 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.5564384151593466E-2"/>
-                  <c:y val="0.12962958929648755"/>
+                  <c:x val="1.0137426900584787E-2"/>
+                  <c:y val="0.25269153746770018"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{F4E1CDFC-9249-4D03-A4CB-69DD38853DC4}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>;</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:fld id="{3A4183CC-E9D7-45E4-BA24-186F39CC189F}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -694,8 +784,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 111592"/>
-                        <a:gd name="adj2" fmla="val -14785"/>
+                        <a:gd name="adj1" fmla="val 126278"/>
+                        <a:gd name="adj2" fmla="val -66323"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -716,6 +806,8 @@
                       <a:noFill/>
                     </a:ln>
                   </c15:spPr>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-12CE-4448-BD84-2EB2E274863D}"/>
@@ -726,14 +818,58 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.3570202940510837E-2"/>
-                  <c:y val="2.8921161855850447E-2"/>
+                  <c:x val="1.1164473684210526E-2"/>
+                  <c:y val="1.2512919896640788E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{2C889CB0-4322-4663-BB7A-266DED9BEB1C}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>;</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:fld id="{09ECA2ED-28C4-4E49-89D0-F36FD0F7E331}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
                 <a:xfrm>
-                  <a:off x="243646" y="536651"/>
-                  <a:ext cx="949124" cy="353900"/>
+                  <a:off x="157861" y="507640"/>
+                  <a:ext cx="944009" cy="376263"/>
                 </a:xfrm>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -791,8 +927,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 103607"/>
-                        <a:gd name="adj2" fmla="val 101456"/>
+                        <a:gd name="adj1" fmla="val 70310"/>
+                        <a:gd name="adj2" fmla="val 129302"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -815,10 +951,12 @@
                   </c15:spPr>
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.23146499754177033"/>
-                      <c:h val="0.12153182369609203"/>
+                      <c:w val="0.27602631578947362"/>
+                      <c:h val="0.12153197674418605"/>
                     </c:manualLayout>
                   </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-12CE-4448-BD84-2EB2E274863D}"/>
@@ -829,11 +967,59 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.17928663542503961"/>
-                  <c:y val="0.14351862943465918"/>
+                  <c:x val="6.2038888888888886E-2"/>
+                  <c:y val="0.13121253229974161"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{D4E35A52-B943-4B5A-B720-5F9CFFC4E6CF}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>;</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:fld id="{554259BA-53E5-437D-AA76-CAB8F2A1B232}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
+                <a:xfrm>
+                  <a:off x="2352413" y="505579"/>
+                  <a:ext cx="859941" cy="628377"/>
+                </a:xfrm>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
                     <a:srgbClr val="000000">
@@ -890,8 +1076,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val -172224"/>
-                        <a:gd name="adj2" fmla="val 54241"/>
+                        <a:gd name="adj1" fmla="val -114627"/>
+                        <a:gd name="adj2" fmla="val 75462"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -912,6 +1098,14 @@
                       <a:noFill/>
                     </a:ln>
                   </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.25144473684210528"/>
+                      <c:h val="0.20296414728682172"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-12CE-4448-BD84-2EB2E274863D}"/>
@@ -922,14 +1116,57 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.5863872609078948E-2"/>
-                  <c:y val="0.17712791405943154"/>
+                  <c:x val="-4.6418128654970761E-2"/>
+                  <c:y val="0.20994444444444438"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{DEB3DE5A-E62D-44D1-93BC-ACEEF2545DB3}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>;</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{8322BF51-D47B-4546-B635-994D2ACDCF07}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
                 <a:xfrm>
-                  <a:off x="3057025" y="1698391"/>
-                  <a:ext cx="923725" cy="334800"/>
+                  <a:off x="2249524" y="1980291"/>
+                  <a:ext cx="1011725" cy="376263"/>
                 </a:xfrm>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -987,8 +1224,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val -101642"/>
-                        <a:gd name="adj2" fmla="val -119340"/>
+                        <a:gd name="adj1" fmla="val -39506"/>
+                        <a:gd name="adj2" fmla="val -134529"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -1011,10 +1248,12 @@
                   </c15:spPr>
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.22527064912869421"/>
-                      <c:h val="0.12153182369609203"/>
+                      <c:w val="0.29582602339181285"/>
+                      <c:h val="0.12153197674418605"/>
                     </c:manualLayout>
                   </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-12CE-4448-BD84-2EB2E274863D}"/>
@@ -1804,6 +2043,81 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.12413893884892084"/>
+                  <c:y val="0.17378165374677002"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:pattFill prst="pct75">
+                  <a:fgClr>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:fgClr>
+                  <a:bgClr>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:bgClr>
+                </a:pattFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>; </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.48862260191846513"/>
+                      <c:h val="0.10697674418604651"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-3FAF-4D1C-844A-631AEE3B0B77}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:pattFill prst="pct75">
                 <a:fgClr>
@@ -2134,6 +2448,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.11736610711430857"/>
+                  <c:y val="0.16967958656330751"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -2179,7 +2499,7 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="ctr"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="1"/>
@@ -2191,8 +2511,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.40553468600023129"/>
-                      <c:h val="0.14074069969650052"/>
+                      <c:w val="0.68345323741007191"/>
+                      <c:h val="0.10697674418604651"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -2584,10 +2904,49 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.24792294230574133"/>
-                  <c:y val="-6.5147301071498326E-2"/>
+                  <c:x val="-0.12448405192497893"/>
+                  <c:y val="-6.514718370996625E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{E14AFB74-3100-4A61-BD9D-7B59E3032975}" type="CATEGORYNAME">
+                      <a:rPr lang="hy-AM"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="hy-AM"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{63B4ED58-534A-42AA-9E6F-3F5C0FE2261C}" type="PERCENTAGE">
+                      <a:rPr lang="hy-AM" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="hy-AM"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -2645,8 +3004,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 154655"/>
-                        <a:gd name="adj2" fmla="val -131541"/>
+                        <a:gd name="adj1" fmla="val 62527"/>
+                        <a:gd name="adj2" fmla="val -171535"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -2667,6 +3026,8 @@
                       <a:noFill/>
                     </a:ln>
                   </c15:spPr>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-BF62-4C06-825B-3F344120A4CB}"/>
@@ -2677,10 +3038,49 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.5564310017870938E-2"/>
-                  <c:y val="0.24488154277172408"/>
+                  <c:x val="5.4792846148363307E-2"/>
+                  <c:y val="0.31247678816853031"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{1847F9A3-B3C6-41FD-9A44-FA2A67933B95}" type="CATEGORYNAME">
+                      <a:rPr lang="hy-AM"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="hy-AM"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{A3D4F1E9-88F9-4490-9010-93FC38143401}" type="PERCENTAGE">
+                      <a:rPr lang="hy-AM" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="hy-AM"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -2738,8 +3138,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 136208"/>
-                        <a:gd name="adj2" fmla="val -63291"/>
+                        <a:gd name="adj1" fmla="val 79736"/>
+                        <a:gd name="adj2" fmla="val -116344"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -2760,6 +3160,8 @@
                       <a:noFill/>
                     </a:ln>
                   </c15:spPr>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-BF62-4C06-825B-3F344120A4CB}"/>
@@ -2770,14 +3172,53 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.2153248179739508E-2"/>
-                  <c:y val="0.11103119099009233"/>
+                  <c:x val="2.0861326234696803E-2"/>
+                  <c:y val="8.602866557694263E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{08A421B5-0EB0-438A-B379-8C60B78A686F}" type="CATEGORYNAME">
+                      <a:rPr lang="hy-AM"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="hy-AM"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{CD3996E1-BB59-461A-ADCE-EC739C96AF5D}" type="PERCENTAGE">
+                      <a:rPr lang="hy-AM" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="hy-AM"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
                 <a:xfrm>
-                  <a:off x="167446" y="624800"/>
-                  <a:ext cx="949124" cy="482399"/>
+                  <a:off x="177800" y="808905"/>
+                  <a:ext cx="938270" cy="331200"/>
                 </a:xfrm>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -2835,8 +3276,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 111636"/>
-                        <a:gd name="adj2" fmla="val 48144"/>
+                        <a:gd name="adj1" fmla="val 74075"/>
+                        <a:gd name="adj2" fmla="val 151527"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -2859,10 +3300,12 @@
                   </c15:spPr>
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.23146499754177033"/>
-                      <c:h val="0.17511036962662721"/>
+                      <c:w val="0.27635171474131465"/>
+                      <c:h val="9.7933230353624126E-2"/>
                     </c:manualLayout>
                   </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-BF62-4C06-825B-3F344120A4CB}"/>
@@ -2873,11 +3316,54 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.17928663542503961"/>
-                  <c:y val="0.14351862943465918"/>
+                  <c:x val="0.10019068062438627"/>
+                  <c:y val="8.9066902116445884E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{6C0140AC-24E6-4FBB-B5A7-CD9228AF5273}" type="CATEGORYNAME">
+                      <a:rPr lang="hy-AM"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="hy-AM"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{940D0FE3-E41C-4C5E-9395-0899B87F4409}" type="PERCENTAGE">
+                      <a:rPr lang="hy-AM" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="hy-AM"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
+                <a:xfrm>
+                  <a:off x="2471172" y="804980"/>
+                  <a:ext cx="771634" cy="488677"/>
+                </a:xfrm>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
                     <a:srgbClr val="000000">
@@ -2934,8 +3420,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val -172224"/>
-                        <a:gd name="adj2" fmla="val 54241"/>
+                        <a:gd name="adj1" fmla="val -127786"/>
+                        <a:gd name="adj2" fmla="val 102970"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -2956,6 +3442,14 @@
                       <a:noFill/>
                     </a:ln>
                   </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.22727162946813831"/>
+                      <c:h val="0.14449793843453496"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-BF62-4C06-825B-3F344120A4CB}"/>
@@ -2966,14 +3460,53 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.7800157638839598E-4"/>
-                  <c:y val="0.22783877358853555"/>
+                  <c:x val="-5.9849093103629056E-2"/>
+                  <c:y val="0.1902860111606034"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{209D3A97-6A35-4E48-A5FC-57F1D33DCF0E}" type="CATEGORYNAME">
+                      <a:rPr lang="hy-AM"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="hy-AM"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{DB82410D-E016-4CF9-9BDF-A4C91B48A1FF}" type="PERCENTAGE">
+                      <a:rPr lang="hy-AM" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="hy-AM"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
                 <a:xfrm>
-                  <a:off x="2993525" y="1748739"/>
-                  <a:ext cx="923725" cy="487200"/>
+                  <a:off x="2427166" y="2116384"/>
+                  <a:ext cx="764840" cy="598097"/>
                 </a:xfrm>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -3031,8 +3564,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val -88237"/>
-                        <a:gd name="adj2" fmla="val -109564"/>
+                        <a:gd name="adj1" fmla="val -50877"/>
+                        <a:gd name="adj2" fmla="val -88861"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -3059,6 +3592,8 @@
                       <c:h val="0.17685276136420564"/>
                     </c:manualLayout>
                   </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-BF62-4C06-825B-3F344120A4CB}"/>
@@ -3414,6 +3949,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.1760735870481224"/>
+                  <c:y val="0.20394006374956408"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -3459,7 +4000,7 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="ctr"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="1"/>
@@ -3471,8 +4012,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.33146063592863617"/>
-                      <c:h val="0.14074069969650052"/>
+                      <c:w val="0.58189930376090726"/>
+                      <c:h val="0.12031714028825982"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -3859,10 +4400,485 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.24792294230574133"/>
-                  <c:y val="-6.5147301071498326E-2"/>
+                  <c:x val="0.1116277389483618"/>
+                  <c:y val="-6.0327332725141174E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{03B89080-9CA1-4F81-9AAF-819E80A50DFA}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>;</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{4545DD8F-922C-49D5-93F7-AC03C3DE24CA}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:xfrm>
+                  <a:off x="1745288" y="2407616"/>
+                  <a:ext cx="750400" cy="331200"/>
+                </a:xfrm>
+                <a:pattFill prst="pct75">
+                  <a:fgClr>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:srgbClr>
+                  </a:fgClr>
+                  <a:bgClr>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:srgbClr>
+                  </a:bgClr>
+                </a:pattFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst>
+                        <a:gd name="adj1" fmla="val -58803"/>
+                        <a:gd name="adj2" fmla="val -153787"/>
+                      </a:avLst>
+                    </a:prstGeom>
+                    <a:pattFill prst="pct75">
+                      <a:fgClr>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:fgClr>
+                      <a:bgClr>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:bgClr>
+                    </a:pattFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.22129847533103303"/>
+                      <c:h val="0.11363289370349569"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-82A8-43BD-89B0-6D0199DB7D8E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.7431802766227252E-2"/>
+                  <c:y val="0.36297852674541597"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{0AFC27C5-11A4-4670-B096-287F283E88D0}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{A2585AC7-DEAC-4422-AD63-0D389474826A}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:xfrm>
+                  <a:off x="194745" y="2105969"/>
+                  <a:ext cx="978834" cy="504000"/>
+                </a:xfrm>
+                <a:pattFill prst="pct75">
+                  <a:fgClr>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:srgbClr>
+                  </a:fgClr>
+                  <a:bgClr>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:srgbClr>
+                  </a:bgClr>
+                </a:pattFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst>
+                        <a:gd name="adj1" fmla="val 50833"/>
+                        <a:gd name="adj2" fmla="val -153956"/>
+                      </a:avLst>
+                    </a:prstGeom>
+                    <a:pattFill prst="pct75">
+                      <a:fgClr>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:fgClr>
+                      <a:bgClr>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:bgClr>
+                    </a:pattFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.28866525111327368"/>
+                      <c:h val="0.17291962085314561"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-82A8-43BD-89B0-6D0199DB7D8E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.8566162375770451E-3"/>
+                  <c:y val="6.2182444609968869E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{561A4B24-934E-4BAC-B722-1332A026DEF2}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{2B246DE7-3D3C-4456-8D79-F1FE6F80ECDA}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:xfrm>
+                  <a:off x="203199" y="737897"/>
+                  <a:ext cx="937275" cy="331200"/>
+                </a:xfrm>
+                <a:pattFill prst="pct75">
+                  <a:fgClr>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:srgbClr>
+                  </a:fgClr>
+                  <a:bgClr>
+                    <a:srgbClr val="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:srgbClr>
+                  </a:bgClr>
+                </a:pattFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="wedgeRectCallout">
+                      <a:avLst>
+                        <a:gd name="adj1" fmla="val 78100"/>
+                        <a:gd name="adj2" fmla="val 137297"/>
+                      </a:avLst>
+                    </a:prstGeom>
+                    <a:pattFill prst="pct75">
+                      <a:fgClr>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:fgClr>
+                      <a:bgClr>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:bgClr>
+                    </a:pattFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.27640891798637535"/>
+                      <c:h val="0.11363289370349569"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-82A8-43BD-89B0-6D0199DB7D8E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15306939160694802"/>
+                  <c:y val="0.10866008222602447"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{8A8D0A78-E3A1-48D1-81A8-723F68CA8286}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>; </a:t>
+                    </a:r>
+                    <a:fld id="{FD7822FF-DCAB-44D7-A8F8-9834F450EECE}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -3920,8 +4936,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 154655"/>
-                        <a:gd name="adj2" fmla="val -131541"/>
+                        <a:gd name="adj1" fmla="val -163765"/>
+                        <a:gd name="adj2" fmla="val 64852"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -3942,117 +4958,70 @@
                       <a:noFill/>
                     </a:ln>
                   </c15:spPr>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-82A8-43BD-89B0-6D0199DB7D8E}"/>
+                  <c16:uniqueId val="{00000007-82A8-43BD-89B0-6D0199DB7D8E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="1"/>
+              <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.5564310017870938E-2"/>
-                  <c:y val="0.24488154277172408"/>
+                  <c:x val="-3.3582529711876037E-2"/>
+                  <c:y val="0.16486983204134359"/>
                 </c:manualLayout>
               </c:layout>
-              <c:spPr>
-                <a:pattFill prst="pct75">
-                  <a:fgClr>
-                    <a:srgbClr val="000000">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:srgbClr>
-                  </a:fgClr>
-                  <a:bgClr>
-                    <a:srgbClr val="000000">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:srgbClr>
-                  </a:bgClr>
-                </a:pattFill>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:prstGeom prst="wedgeRectCallout">
-                      <a:avLst>
-                        <a:gd name="adj1" fmla="val 136208"/>
-                        <a:gd name="adj2" fmla="val -63291"/>
-                      </a:avLst>
-                    </a:prstGeom>
-                    <a:pattFill prst="pct75">
-                      <a:fgClr>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:fgClr>
-                      <a:bgClr>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:bgClr>
-                    </a:pattFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                  </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-82A8-43BD-89B0-6D0199DB7D8E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-9.2153248179739508E-2"/>
-                  <c:y val="0.11103119099009233"/>
-                </c:manualLayout>
-              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="lt1"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{379E4230-BA91-4A5D-BD00-2C706B4AC3D1}" type="CATEGORYNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[CATEGORY NAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>;</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>
+</a:t>
+                    </a:r>
+                    <a:fld id="{DCC1244A-F9DF-4738-8AE9-4BAEA741DF88}" type="PERCENTAGE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[PERCENTAGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:spPr>
                 <a:xfrm>
-                  <a:off x="167446" y="624800"/>
-                  <a:ext cx="949124" cy="482399"/>
+                  <a:off x="2588794" y="1811098"/>
+                  <a:ext cx="713206" cy="504000"/>
                 </a:xfrm>
                 <a:pattFill prst="pct75">
                   <a:fgClr>
@@ -4110,8 +5079,8 @@
                   <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <a:prstGeom prst="wedgeRectCallout">
                       <a:avLst>
-                        <a:gd name="adj1" fmla="val 111636"/>
-                        <a:gd name="adj2" fmla="val 48144"/>
+                        <a:gd name="adj1" fmla="val -95747"/>
+                        <a:gd name="adj2" fmla="val -69877"/>
                       </a:avLst>
                     </a:prstGeom>
                     <a:pattFill prst="pct75">
@@ -4134,206 +5103,12 @@
                   </c15:spPr>
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.23146499754177033"/>
-                      <c:h val="0.17511036962662721"/>
+                      <c:w val="0.21032941107080716"/>
+                      <c:h val="0.17291962085314561"/>
                     </c:manualLayout>
                   </c15:layout>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-82A8-43BD-89B0-6D0199DB7D8E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.17928663542503961"/>
-                  <c:y val="0.14351862943465918"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:spPr>
-                <a:pattFill prst="pct75">
-                  <a:fgClr>
-                    <a:srgbClr val="000000">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:srgbClr>
-                  </a:fgClr>
-                  <a:bgClr>
-                    <a:srgbClr val="000000">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:srgbClr>
-                  </a:bgClr>
-                </a:pattFill>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:prstGeom prst="wedgeRectCallout">
-                      <a:avLst>
-                        <a:gd name="adj1" fmla="val -172224"/>
-                        <a:gd name="adj2" fmla="val 54241"/>
-                      </a:avLst>
-                    </a:prstGeom>
-                    <a:pattFill prst="pct75">
-                      <a:fgClr>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:fgClr>
-                      <a:bgClr>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:bgClr>
-                    </a:pattFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                  </c15:spPr>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-82A8-43BD-89B0-6D0199DB7D8E}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="5.3029963087536387E-2"/>
-                  <c:y val="0.22783877358853555"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:spPr>
-                <a:xfrm>
-                  <a:off x="3206885" y="1748739"/>
-                  <a:ext cx="669725" cy="487200"/>
-                </a:xfrm>
-                <a:pattFill prst="pct75">
-                  <a:fgClr>
-                    <a:srgbClr val="000000">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:srgbClr>
-                  </a:fgClr>
-                  <a:bgClr>
-                    <a:srgbClr val="000000">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:srgbClr>
-                  </a:bgClr>
-                </a:pattFill>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:noAutofit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:prstGeom prst="wedgeRectCallout">
-                      <a:avLst>
-                        <a:gd name="adj1" fmla="val -123793"/>
-                        <a:gd name="adj2" fmla="val -109564"/>
-                      </a:avLst>
-                    </a:prstGeom>
-                    <a:pattFill prst="pct75">
-                      <a:fgClr>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:fgClr>
-                      <a:bgClr>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:bgClr>
-                    </a:pattFill>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                  </c15:spPr>
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="0.16332716499793196"/>
-                      <c:h val="0.17685276136420561"/>
-                    </c:manualLayout>
-                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-82A8-43BD-89B0-6D0199DB7D8E}"/>
@@ -9027,16 +9802,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>319088</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>57146</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>509588</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>142871</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>59255</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>271988</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>371</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9101,16 +9876,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>218210</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>106506</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>561976</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>387546</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>125931</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9137,16 +9912,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>422462</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>438380</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>17192</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9177,14 +9952,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>156881</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>442912</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>2109</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>347206</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>138352</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9213,16 +9988,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>38101</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>19425</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9251,16 +10026,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>2109</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>38474</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11512,8 +12287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E454DF-89F0-409B-9508-3615242338D2}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>